<commit_message>
add height and low tick over up +1-2% over down 0,2%
</commit_message>
<xml_diff>
--- a/history/summary.xlsx
+++ b/history/summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pavel.rostov\PycharmProjects\scrapyBotTrade\history\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0242503-C16A-4908-83C3-C8E1D79BD325}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81852167-EF44-4E42-A8CB-550DD09C6846}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,6 +21,7 @@
     <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -80,7 +81,8 @@
     <t>goal more 1%</t>
   </si>
   <si>
-    <t>goal more 0,5%</t>
+    <t>goal 
+more 0,5%</t>
   </si>
 </sst>
 </file>
@@ -138,7 +140,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -236,13 +238,43 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -251,105 +283,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -366,7 +299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -407,7 +340,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -419,7 +352,7 @@
     <xf numFmtId="10" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="1" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -428,47 +361,29 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -750,8 +665,62 @@
           </cell>
         </row>
         <row r="5">
-          <cell r="AA5">
-            <v>0.23846153846153847</v>
+          <cell r="Z5">
+            <v>31</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="Z1">
+            <v>30</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="U2">
+            <v>124</v>
+          </cell>
+          <cell r="Z2">
+            <v>24</v>
+          </cell>
+          <cell r="AD2">
+            <v>3767.6899999999991</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="J3">
+            <v>44267</v>
+          </cell>
+          <cell r="Z3">
+            <v>18</v>
+          </cell>
+          <cell r="AD3">
+            <v>3822.6141464907637</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="Z4">
+            <v>22</v>
+          </cell>
+          <cell r="AD4">
+            <v>1.4368216196025463E-2</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="Z5">
+            <v>30</v>
           </cell>
         </row>
       </sheetData>
@@ -1023,17 +992,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:R8"/>
+  <dimension ref="B2:R9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R19" sqref="R19"/>
+      <selection activeCell="S19" sqref="S19:S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.5703125" customWidth="1"/>
+    <col min="18" max="18" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1044,22 +1013,22 @@
       <c r="C3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="31" t="s">
+      <c r="E3" s="26"/>
+      <c r="F3" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="32"/>
-      <c r="H3" s="31" t="s">
+      <c r="G3" s="27"/>
+      <c r="H3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="31" t="s">
+      <c r="I3" s="27"/>
+      <c r="J3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="33"/>
+      <c r="K3" s="28"/>
       <c r="L3" s="11" t="s">
         <v>9</v>
       </c>
@@ -1093,31 +1062,31 @@
         <f>[1]Sheet1!$V$1</f>
         <v>37</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="23">
         <f>D4/C4</f>
         <v>0.40217391304347827</v>
       </c>
-      <c r="F4" s="22">
+      <c r="F4" s="21">
         <f>[1]Sheet1!$V$2</f>
         <v>16</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4" s="23">
         <f>F4/C4</f>
         <v>0.17391304347826086</v>
       </c>
-      <c r="H4" s="22">
+      <c r="H4" s="21">
         <f>[1]Sheet1!$V$3</f>
         <v>13</v>
       </c>
-      <c r="I4" s="25">
+      <c r="I4" s="23">
         <f>H4/C4</f>
         <v>0.14130434782608695</v>
       </c>
-      <c r="J4" s="22">
+      <c r="J4" s="21">
         <f>[1]Sheet1!$V$4</f>
         <v>13</v>
       </c>
-      <c r="K4" s="27">
+      <c r="K4" s="24">
         <f>J4/C4</f>
         <v>0.14130434782608695</v>
       </c>
@@ -1163,31 +1132,31 @@
         <f>[2]Sheet1!$Z$1</f>
         <v>35</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="23">
         <f t="shared" ref="E5:E7" si="0">D5/C5</f>
         <v>0.4861111111111111</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F5" s="21">
         <f>[2]Sheet1!$Z$2</f>
         <v>12</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="23">
         <f t="shared" ref="G5:G7" si="1">F5/C5</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="H5" s="22">
+      <c r="H5" s="21">
         <f>[2]Sheet1!$Z$3</f>
         <v>11</v>
       </c>
-      <c r="I5" s="25">
+      <c r="I5" s="23">
         <f t="shared" ref="I5:I7" si="2">H5/C5</f>
         <v>0.15277777777777779</v>
       </c>
-      <c r="J5" s="22">
+      <c r="J5" s="21">
         <f>[2]Sheet1!$Z$4</f>
         <v>7</v>
       </c>
-      <c r="K5" s="27">
+      <c r="K5" s="24">
         <f t="shared" ref="K5:K7" si="3">J5/C5</f>
         <v>9.7222222222222224E-2</v>
       </c>
@@ -1233,31 +1202,31 @@
         <f>[3]Sheet1!$Z$1</f>
         <v>18</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="23">
         <f t="shared" si="0"/>
         <v>0.28125</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="22">
         <f>[3]Sheet1!$Z$2</f>
         <v>9</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="23">
         <f t="shared" si="1"/>
         <v>0.140625</v>
       </c>
-      <c r="H6" s="23">
+      <c r="H6" s="22">
         <f>[3]Sheet1!$Z$3</f>
         <v>9</v>
       </c>
-      <c r="I6" s="25">
+      <c r="I6" s="23">
         <f t="shared" si="2"/>
         <v>0.140625</v>
       </c>
-      <c r="J6" s="23">
+      <c r="J6" s="22">
         <f>[3]Sheet1!$Z$4</f>
         <v>13</v>
       </c>
-      <c r="K6" s="27">
+      <c r="K6" s="24">
         <f t="shared" si="3"/>
         <v>0.203125</v>
       </c>
@@ -1303,31 +1272,31 @@
         <f>[4]Sheet1!$Z$1</f>
         <v>79</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="23">
         <f t="shared" si="0"/>
         <v>0.68695652173913047</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="22">
         <f>[4]Sheet1!$Z$2</f>
         <v>13</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="23">
         <f t="shared" si="1"/>
         <v>0.11304347826086956</v>
       </c>
-      <c r="H7" s="23">
+      <c r="H7" s="22">
         <f>[4]Sheet1!$Z$3</f>
         <v>9</v>
       </c>
-      <c r="I7" s="25">
+      <c r="I7" s="23">
         <f t="shared" si="2"/>
         <v>7.8260869565217397E-2</v>
       </c>
-      <c r="J7" s="23">
+      <c r="J7" s="22">
         <f>[4]Sheet1!$Z$4</f>
         <v>6</v>
       </c>
-      <c r="K7" s="27">
+      <c r="K7" s="24">
         <f t="shared" si="3"/>
         <v>5.2173913043478258E-2</v>
       </c>
@@ -1360,7 +1329,7 @@
         <v>0.93043478260869561</v>
       </c>
     </row>
-    <row r="8" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="6">
         <f>[5]Sheet1!$J$3</f>
         <v>44266</v>
@@ -1369,45 +1338,45 @@
         <f>[5]Sheet1!$U$2</f>
         <v>130</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="20">
         <f>[5]Sheet1!$Z$1</f>
         <v>30</v>
       </c>
-      <c r="E8" s="26">
-        <f t="shared" ref="E8" si="7">D8/C8</f>
+      <c r="E8" s="23">
+        <f t="shared" ref="E8:E9" si="7">D8/C8</f>
         <v>0.23076923076923078</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="22">
         <f>[5]Sheet1!$Z$2</f>
         <v>20</v>
       </c>
-      <c r="G8" s="26">
-        <f t="shared" ref="G8" si="8">F8/C8</f>
+      <c r="G8" s="23">
+        <f t="shared" ref="G8:G9" si="8">F8/C8</f>
         <v>0.15384615384615385</v>
       </c>
-      <c r="H8" s="24">
+      <c r="H8" s="22">
         <f>[5]Sheet1!$Z$3</f>
         <v>23</v>
       </c>
-      <c r="I8" s="26">
-        <f t="shared" ref="I8" si="9">H8/C8</f>
+      <c r="I8" s="23">
+        <f t="shared" ref="I8:I9" si="9">H8/C8</f>
         <v>0.17692307692307693</v>
       </c>
-      <c r="J8" s="24">
+      <c r="J8" s="22">
         <f>[5]Sheet1!$Z$4</f>
         <v>26</v>
       </c>
-      <c r="K8" s="28">
-        <f t="shared" ref="K8" si="10">J8/C8</f>
+      <c r="K8" s="24">
+        <f t="shared" ref="K8:K9" si="10">J8/C8</f>
         <v>0.2</v>
       </c>
-      <c r="L8" s="34">
-        <f>[5]Sheet1!$AA$5</f>
+      <c r="L8" s="13">
+        <f>[5]Sheet1!$Z$5</f>
+        <v>31</v>
+      </c>
+      <c r="M8" s="8">
+        <f t="shared" ref="M8:M9" si="11">L8/C8</f>
         <v>0.23846153846153847</v>
-      </c>
-      <c r="M8" s="8">
-        <f t="shared" ref="M8" si="11">L8/C8</f>
-        <v>1.8343195266272191E-3</v>
       </c>
       <c r="N8" s="7">
         <f>[5]Sheet1!$AD$2</f>
@@ -1428,6 +1397,76 @@
       <c r="R8" s="18">
         <f t="shared" si="6"/>
         <v>0.7615384615384615</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="6">
+        <f>[6]Sheet1!$J$3</f>
+        <v>44267</v>
+      </c>
+      <c r="C9" s="10">
+        <f>[6]Sheet1!$U$2</f>
+        <v>124</v>
+      </c>
+      <c r="D9" s="20">
+        <f>[6]Sheet1!$Z$1</f>
+        <v>30</v>
+      </c>
+      <c r="E9" s="23">
+        <f t="shared" ref="E9" si="12">D9/C9</f>
+        <v>0.24193548387096775</v>
+      </c>
+      <c r="F9" s="22">
+        <f>[6]Sheet1!$Z$2</f>
+        <v>24</v>
+      </c>
+      <c r="G9" s="23">
+        <f t="shared" ref="G9" si="13">F9/C9</f>
+        <v>0.19354838709677419</v>
+      </c>
+      <c r="H9" s="22">
+        <f>[6]Sheet1!$Z$3</f>
+        <v>18</v>
+      </c>
+      <c r="I9" s="23">
+        <f t="shared" ref="I9" si="14">H9/C9</f>
+        <v>0.14516129032258066</v>
+      </c>
+      <c r="J9" s="22">
+        <f>[6]Sheet1!$Z$4</f>
+        <v>22</v>
+      </c>
+      <c r="K9" s="24">
+        <f t="shared" ref="K9" si="15">J9/C9</f>
+        <v>0.17741935483870969</v>
+      </c>
+      <c r="L9" s="13">
+        <f>[6]Sheet1!$Z$5</f>
+        <v>30</v>
+      </c>
+      <c r="M9" s="8">
+        <f t="shared" ref="M9" si="16">L9/C9</f>
+        <v>0.24193548387096775</v>
+      </c>
+      <c r="N9" s="7">
+        <f>[6]Sheet1!$AD$2</f>
+        <v>3767.6899999999991</v>
+      </c>
+      <c r="O9" s="15">
+        <f>[6]Sheet1!$AD$3</f>
+        <v>3822.6141464907637</v>
+      </c>
+      <c r="P9" s="17">
+        <f>[6]Sheet1!$AD$4</f>
+        <v>1.4368216196025463E-2</v>
+      </c>
+      <c r="Q9" s="18">
+        <f t="shared" ref="Q9" si="17">(D9+F9+H9)/C9</f>
+        <v>0.58064516129032262</v>
+      </c>
+      <c r="R9" s="18">
+        <f t="shared" ref="R9" si="18">(D9+F9+H9+J9)/C9</f>
+        <v>0.75806451612903225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>